<commit_message>
completed Nopcommerce place order feature Test
</commit_message>
<xml_diff>
--- a/Test/TestData/test_data.xlsx
+++ b/Test/TestData/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdullah.faroque\PycharmProjects\nopCommerce-Web-UI-Automation\Test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32634AA4-B7EE-44F9-AC98-16211396B282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E558D7-2109-4F4C-82F1-35D44EEB192C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
     <t>Your registration completed</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>